<commit_message>
updating reports for continuity
</commit_message>
<xml_diff>
--- a/xls/templates/campaign-plan.xlsx
+++ b/xls/templates/campaign-plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B0982A-30F2-3C4A-BB73-CDF70E86EB64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5067BBA-5F1F-9A42-83B5-2C48660BB7B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" xr2:uid="{4E81CDE1-BD59-C741-94CA-47E4A75CBD89}"/>
+    <workbookView xWindow="25620" yWindow="460" windowWidth="38380" windowHeight="21140" activeTab="7" xr2:uid="{4E81CDE1-BD59-C741-94CA-47E4A75CBD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="91">
   <si>
     <t>Tactic</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Weekly</t>
   </si>
   <si>
-    <t>Daily</t>
-  </si>
-  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -308,6 +305,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Number of Weeks in Campaign</t>
+  </si>
+  <si>
+    <t>Number of Days in Campaign</t>
   </si>
 </sst>
 </file>
@@ -317,9 +320,9 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,8 +345,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +371,26 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
       </patternFill>
     </fill>
   </fills>
@@ -389,13 +427,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
@@ -404,9 +446,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="8">
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="6" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="7" builtinId="41"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CE0F1F-D1AE-0E40-8CEE-85761A5E708F}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,277 +789,309 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>55</v>
-      </c>
+      <c r="A12" s="11"/>
       <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
       <c r="B13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
       <c r="B14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>59</v>
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>61</v>
-      </c>
+      <c r="A17" s="11"/>
       <c r="B17" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
       <c r="B18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="11"/>
       <c r="B19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>65</v>
       </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>66</v>
-      </c>
+      <c r="A22" s="11"/>
       <c r="B22" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
       <c r="B23" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="A24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>69</v>
       </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
+      <c r="A26" s="11"/>
       <c r="B26" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
       <c r="B27" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
         <v>73</v>
       </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>74</v>
-      </c>
+      <c r="A30" s="11"/>
       <c r="B30" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="11"/>
       <c r="B31" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" t="s">
+    <row r="35" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D36" t="s">
-        <v>87</v>
+    </row>
+    <row r="36" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="7">
+        <f>SUM(C36:D36)</f>
+        <v>20000</v>
+      </c>
+      <c r="C36" s="8">
+        <f>SUMIF('Reputation Building'!B2:B48, "Acquisition", 'Reputation Building'!I2:I48)</f>
+        <v>15000</v>
+      </c>
+      <c r="D36" s="8">
+        <f>SUMIF('Reputation Building'!B2:B48, "Retention", 'Reputation Building'!I2:I48)</f>
+        <v>5000</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B37" s="7">
-        <f>SUM(C37:D37)</f>
-        <v>20000</v>
+        <f t="shared" ref="B37:B39" si="0">SUM(C37:D37)</f>
+        <v>15000</v>
       </c>
       <c r="C37" s="8">
-        <f>SUMIF('Reputation Building'!B2:B48, "Acquisition", 'Reputation Building'!I2:I48)</f>
-        <v>15000</v>
+        <f>SUMIF('Demand Creation'!B2:B48, "Acquisition", 'Demand Creation'!I2:I48)</f>
+        <v>5000</v>
       </c>
       <c r="D37" s="8">
-        <f>SUMIF('Reputation Building'!B2:B48, "Retention", 'Reputation Building'!I2:I48)</f>
-        <v>5000</v>
+        <f>SUMIF('Demand Creation'!B2:B48, "Retention", 'Demand Creation'!I2:I48)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B38" s="7">
-        <f t="shared" ref="B38:B40" si="0">SUM(C38:D38)</f>
-        <v>15000</v>
+        <f t="shared" si="0"/>
+        <v>20000</v>
       </c>
       <c r="C38" s="8">
-        <f>SUMIF('Demand Creation'!B2:B48, "Acquisition", 'Demand Creation'!I2:I48)</f>
-        <v>5000</v>
+        <f>SUMIF('Leasing Enablement'!B2:B48, "Acquisition", 'Leasing Enablement'!I2:I48)</f>
+        <v>10000</v>
       </c>
       <c r="D38" s="8">
-        <f>SUMIF('Demand Creation'!B2:B48, "Retention", 'Demand Creation'!I2:I48)</f>
+        <f>SUMIF('Leasing Enablement'!B2:B48, "Retention", 'Leasing Enablement'!I2:I48)</f>
         <v>10000</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B39" s="7">
         <f t="shared" si="0"/>
+        <v>20500</v>
+      </c>
+      <c r="C39" s="8">
+        <f>SUMIF('Market Intelligence'!B2:B48, "Acquisition", 'Market Intelligence'!I2:I48)</f>
         <v>20000</v>
       </c>
-      <c r="C39" s="8">
-        <f>SUMIF('Leasing Enablement'!B2:B48, "Acquisition", 'Leasing Enablement'!I2:I48)</f>
-        <v>10000</v>
-      </c>
       <c r="D39" s="8">
-        <f>SUMIF('Leasing Enablement'!B2:B48, "Retention", 'Leasing Enablement'!I2:I48)</f>
-        <v>10000</v>
+        <f>SUMIF('Market Intelligence'!B2:B48, "Retention", 'Market Intelligence'!I2:I48)</f>
+        <v>500</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B40" s="7">
-        <f t="shared" si="0"/>
-        <v>22500</v>
-      </c>
-      <c r="C40" s="8">
-        <f>SUMIF('Market Intelligence'!B2:B48, "Acquisition", 'Market Intelligence'!I2:I48)</f>
-        <v>20000</v>
-      </c>
-      <c r="D40" s="8">
-        <f>SUMIF('Market Intelligence'!B2:B48, "Retention", 'Market Intelligence'!I2:I48)</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41" s="7">
-        <f>SUM(B37:B40)</f>
-        <v>77500</v>
-      </c>
-      <c r="C41" s="7">
-        <f t="shared" ref="C41:D41" si="1">SUM(C37:C40)</f>
+        <f>SUM(B36:B39)</f>
+        <v>75500</v>
+      </c>
+      <c r="C40" s="7">
+        <f t="shared" ref="C40:D40" si="1">SUM(C36:C39)</f>
         <v>50000</v>
       </c>
-      <c r="D41" s="7">
-        <f t="shared" si="1"/>
-        <v>27500</v>
+      <c r="D40" s="7">
+        <f t="shared" si="1"/>
+        <v>25500</v>
       </c>
     </row>
   </sheetData>
@@ -1021,7 +1104,7 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -1061,21 +1144,21 @@
         <v>13</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="3">
         <v>43485</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1">
         <v>15000</v>
@@ -1084,22 +1167,22 @@
         <v>14</v>
       </c>
       <c r="I2" s="1">
-        <f>IF(H2="One-Time", G2, G2*META!$B$1)</f>
+        <f>IF(H2="One-Time", G2,IF(H2="Weekly", G2*META!$B$2, G2*META!$B$1))</f>
         <v>15000</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="3">
         <v>43497</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1">
         <v>5000</v>
@@ -1108,19 +1191,19 @@
         <v>14</v>
       </c>
       <c r="I3" s="1">
-        <f>IF(H3="One-Time", G3, G3*META!$B$1)</f>
+        <f>IF(H3="One-Time", G3,IF(H3="Weekly", G3*META!$B$2, G3*META!$B$1))</f>
         <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3">
         <v>43497</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1">
         <v>5000</v>
@@ -1129,19 +1212,19 @@
         <v>14</v>
       </c>
       <c r="I4" s="1">
-        <f>IF(H4="One-Time", G4, G4*META!$B$1)</f>
+        <f>IF(H4="One-Time", G4,IF(H4="Weekly", G4*META!$B$2, G4*META!$B$1))</f>
         <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3">
         <v>43511</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1">
         <v>10000</v>
@@ -1150,265 +1233,265 @@
         <v>14</v>
       </c>
       <c r="I5" s="1">
-        <f>IF(H5="One-Time", G5, G5*META!$B$1)</f>
+        <f>IF(H5="One-Time", G5,IF(H5="Weekly", G5*META!$B$2, G5*META!$B$1))</f>
         <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I6" s="1">
-        <f>IF(H6="One-Time", G6, G6*META!$B$1)</f>
+        <f>IF(H6="One-Time", G6,IF(H6="Weekly", G6*META!$B$2, G6*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I7" s="1">
-        <f>IF(H7="One-Time", G7, G7*META!$B$1)</f>
+        <f>IF(H7="One-Time", G7,IF(H7="Weekly", G7*META!$B$2, G7*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I8" s="1">
-        <f>IF(H8="One-Time", G8, G8*META!$B$1)</f>
+        <f>IF(H8="One-Time", G8,IF(H8="Weekly", G8*META!$B$2, G8*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I9" s="1">
-        <f>IF(H9="One-Time", G9, G9*META!$B$1)</f>
+        <f>IF(H9="One-Time", G9,IF(H9="Weekly", G9*META!$B$2, G9*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I10" s="1">
-        <f>IF(H10="One-Time", G10, G10*META!$B$1)</f>
+        <f>IF(H10="One-Time", G10,IF(H10="Weekly", G10*META!$B$2, G10*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I11" s="1">
-        <f>IF(H11="One-Time", G11, G11*META!$B$1)</f>
+        <f>IF(H11="One-Time", G11,IF(H11="Weekly", G11*META!$B$2, G11*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I12" s="1">
-        <f>IF(H12="One-Time", G12, G12*META!$B$1)</f>
+        <f>IF(H12="One-Time", G12,IF(H12="Weekly", G12*META!$B$2, G12*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I13" s="1">
-        <f>IF(H13="One-Time", G13, G13*META!$B$1)</f>
+        <f>IF(H13="One-Time", G13,IF(H13="Weekly", G13*META!$B$2, G13*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I14" s="1">
-        <f>IF(H14="One-Time", G14, G14*META!$B$1)</f>
+        <f>IF(H14="One-Time", G14,IF(H14="Weekly", G14*META!$B$2, G14*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I15" s="1">
-        <f>IF(H15="One-Time", G15, G15*META!$B$1)</f>
+        <f>IF(H15="One-Time", G15,IF(H15="Weekly", G15*META!$B$2, G15*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I16" s="1">
-        <f>IF(H16="One-Time", G16, G16*META!$B$1)</f>
+        <f>IF(H16="One-Time", G16,IF(H16="Weekly", G16*META!$B$2, G16*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I17" s="1">
-        <f>IF(H17="One-Time", G17, G17*META!$B$1)</f>
+        <f>IF(H17="One-Time", G17,IF(H17="Weekly", G17*META!$B$2, G17*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I18" s="1">
-        <f>IF(H18="One-Time", G18, G18*META!$B$1)</f>
+        <f>IF(H18="One-Time", G18,IF(H18="Weekly", G18*META!$B$2, G18*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I19" s="1">
-        <f>IF(H19="One-Time", G19, G19*META!$B$1)</f>
+        <f>IF(H19="One-Time", G19,IF(H19="Weekly", G19*META!$B$2, G19*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I20" s="1">
-        <f>IF(H20="One-Time", G20, G20*META!$B$1)</f>
+        <f>IF(H20="One-Time", G20,IF(H20="Weekly", G20*META!$B$2, G20*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I21" s="1">
-        <f>IF(H21="One-Time", G21, G21*META!$B$1)</f>
+        <f>IF(H21="One-Time", G21,IF(H21="Weekly", G21*META!$B$2, G21*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I22" s="1">
-        <f>IF(H22="One-Time", G22, G22*META!$B$1)</f>
+        <f>IF(H22="One-Time", G22,IF(H22="Weekly", G22*META!$B$2, G22*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I23" s="1">
-        <f>IF(H23="One-Time", G23, G23*META!$B$1)</f>
+        <f>IF(H23="One-Time", G23,IF(H23="Weekly", G23*META!$B$2, G23*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I24" s="1">
-        <f>IF(H24="One-Time", G24, G24*META!$B$1)</f>
+        <f>IF(H24="One-Time", G24,IF(H24="Weekly", G24*META!$B$2, G24*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I25" s="1">
-        <f>IF(H25="One-Time", G25, G25*META!$B$1)</f>
+        <f>IF(H25="One-Time", G25,IF(H25="Weekly", G25*META!$B$2, G25*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I26" s="1">
-        <f>IF(H26="One-Time", G26, G26*META!$B$1)</f>
+        <f>IF(H26="One-Time", G26,IF(H26="Weekly", G26*META!$B$2, G26*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I27" s="1">
-        <f>IF(H27="One-Time", G27, G27*META!$B$1)</f>
+        <f>IF(H27="One-Time", G27,IF(H27="Weekly", G27*META!$B$2, G27*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I28" s="1">
-        <f>IF(H28="One-Time", G28, G28*META!$B$1)</f>
+        <f>IF(H28="One-Time", G28,IF(H28="Weekly", G28*META!$B$2, G28*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I29" s="1">
-        <f>IF(H29="One-Time", G29, G29*META!$B$1)</f>
+        <f>IF(H29="One-Time", G29,IF(H29="Weekly", G29*META!$B$2, G29*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I30" s="1">
-        <f>IF(H30="One-Time", G30, G30*META!$B$1)</f>
+        <f>IF(H30="One-Time", G30,IF(H30="Weekly", G30*META!$B$2, G30*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I31" s="1">
-        <f>IF(H31="One-Time", G31, G31*META!$B$1)</f>
+        <f>IF(H31="One-Time", G31,IF(H31="Weekly", G31*META!$B$2, G31*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I32" s="1">
-        <f>IF(H32="One-Time", G32, G32*META!$B$1)</f>
+        <f>IF(H32="One-Time", G32,IF(H32="Weekly", G32*META!$B$2, G32*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I33" s="1">
-        <f>IF(H33="One-Time", G33, G33*META!$B$1)</f>
+        <f>IF(H33="One-Time", G33,IF(H33="Weekly", G33*META!$B$2, G33*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I34" s="1">
-        <f>IF(H34="One-Time", G34, G34*META!$B$1)</f>
+        <f>IF(H34="One-Time", G34,IF(H34="Weekly", G34*META!$B$2, G34*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I35" s="1">
-        <f>IF(H35="One-Time", G35, G35*META!$B$1)</f>
+        <f>IF(H35="One-Time", G35,IF(H35="Weekly", G35*META!$B$2, G35*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I36" s="1">
-        <f>IF(H36="One-Time", G36, G36*META!$B$1)</f>
+        <f>IF(H36="One-Time", G36,IF(H36="Weekly", G36*META!$B$2, G36*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I37" s="1">
-        <f>IF(H37="One-Time", G37, G37*META!$B$1)</f>
+        <f>IF(H37="One-Time", G37,IF(H37="Weekly", G37*META!$B$2, G37*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I38" s="1">
-        <f>IF(H38="One-Time", G38, G38*META!$B$1)</f>
+        <f>IF(H38="One-Time", G38,IF(H38="Weekly", G38*META!$B$2, G38*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I39" s="1">
-        <f>IF(H39="One-Time", G39, G39*META!$B$1)</f>
+        <f>IF(H39="One-Time", G39,IF(H39="Weekly", G39*META!$B$2, G39*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I40" s="1">
-        <f>IF(H40="One-Time", G40, G40*META!$B$1)</f>
+        <f>IF(H40="One-Time", G40,IF(H40="Weekly", G40*META!$B$2, G40*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I41" s="1">
-        <f>IF(H41="One-Time", G41, G41*META!$B$1)</f>
+        <f>IF(H41="One-Time", G41,IF(H41="Weekly", G41*META!$B$2, G41*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I42" s="1">
-        <f>IF(H42="One-Time", G42, G42*META!$B$1)</f>
+        <f>IF(H42="One-Time", G42,IF(H42="Weekly", G42*META!$B$2, G42*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I43" s="1">
-        <f>IF(H43="One-Time", G43, G43*META!$B$1)</f>
+        <f>IF(H43="One-Time", G43,IF(H43="Weekly", G43*META!$B$2, G43*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I44" s="1">
-        <f>IF(H44="One-Time", G44, G44*META!$B$1)</f>
+        <f>IF(H44="One-Time", G44,IF(H44="Weekly", G44*META!$B$2, G44*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I45" s="1">
-        <f>IF(H45="One-Time", G45, G45*META!$B$1)</f>
+        <f>IF(H45="One-Time", G45,IF(H45="Weekly", G45*META!$B$2, G45*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I46" s="1">
-        <f>IF(H46="One-Time", G46, G46*META!$B$1)</f>
+        <f>IF(H46="One-Time", G46,IF(H46="Weekly", G46*META!$B$2, G46*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I47" s="1">
-        <f>IF(H47="One-Time", G47, G47*META!$B$1)</f>
+        <f>IF(H47="One-Time", G47,IF(H47="Weekly", G47*META!$B$2, G47*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I48" s="1">
-        <f>IF(H48="One-Time", G48, G48*META!$B$1)</f>
+        <f>IF(H48="One-Time", G48,IF(H48="Weekly", G48*META!$B$2, G48*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -1445,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2E21A5-54B8-4140-B44A-A65B92B09B00}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1465,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -1486,30 +1569,30 @@
         <v>13</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3">
         <v>43648</v>
@@ -1521,10 +1604,10 @@
         <v>1000</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1">
-        <f>IF(H2="One-Time", G2, G2*META!$B$1)</f>
+        <f>IF(H2="One-Time", G2,IF(H2="Weekly", G2*META!$B$2, G2*META!$B$1))</f>
         <v>5000</v>
       </c>
       <c r="J2">
@@ -1544,10 +1627,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="3">
         <v>43649</v>
@@ -1559,10 +1642,10 @@
         <v>2000</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1">
-        <f>IF(H3="One-Time", G3, G3*META!$B$1)</f>
+        <f>IF(H3="One-Time", G3,IF(H3="Weekly", G3*META!$B$2, G3*META!$B$1))</f>
         <v>10000</v>
       </c>
       <c r="J3">
@@ -1582,7 +1665,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3">
         <v>43650</v>
@@ -1594,10 +1677,10 @@
         <v>1000</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" s="1">
-        <f>IF(H4="One-Time", G4, G4*META!$B$1)</f>
+        <f>IF(H4="One-Time", G4,IF(H4="Weekly", G4*META!$B$2, G4*META!$B$1))</f>
         <v>5000</v>
       </c>
       <c r="J4">
@@ -1617,7 +1700,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>43651</v>
@@ -1629,10 +1712,10 @@
         <v>1000</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1">
-        <f>IF(H5="One-Time", G5, G5*META!$B$1)</f>
+        <f>IF(H5="One-Time", G5,IF(H5="Weekly", G5*META!$B$2, G5*META!$B$1))</f>
         <v>5000</v>
       </c>
       <c r="J5">
@@ -1652,7 +1735,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3">
         <v>43652</v>
@@ -1664,10 +1747,10 @@
         <v>1000</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="1">
-        <f>IF(H6="One-Time", G6, G6*META!$B$1)</f>
+        <f>IF(H6="One-Time", G6,IF(H6="Weekly", G6*META!$B$2, G6*META!$B$1))</f>
         <v>5000</v>
       </c>
       <c r="J6">
@@ -1687,7 +1770,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3">
         <v>43653</v>
@@ -1699,10 +1782,10 @@
         <v>1000</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="1">
-        <f>IF(H7="One-Time", G7, G7*META!$B$1)</f>
+        <f>IF(H7="One-Time", G7,IF(H7="Weekly", G7*META!$B$2, G7*META!$B$1))</f>
         <v>5000</v>
       </c>
       <c r="J7">
@@ -1722,7 +1805,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>43654</v>
@@ -1734,10 +1817,10 @@
         <v>1000</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" s="1">
-        <f>IF(H8="One-Time", G8, G8*META!$B$1)</f>
+        <f>IF(H8="One-Time", G8,IF(H8="Weekly", G8*META!$B$2, G8*META!$B$1))</f>
         <v>5000</v>
       </c>
       <c r="J8">
@@ -1757,13 +1840,13 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3">
         <v>43518</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4">
         <v>2000</v>
@@ -1772,7 +1855,7 @@
         <v>14</v>
       </c>
       <c r="I9" s="1">
-        <f>IF(H9="One-Time", G9, G9*META!$B$1)</f>
+        <f>IF(H9="One-Time", G9,IF(H9="Weekly", G9*META!$B$2, G9*META!$B$1))</f>
         <v>2000</v>
       </c>
       <c r="J9">
@@ -1792,10 +1875,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3">
         <v>43654</v>
@@ -1807,10 +1890,10 @@
         <v>200</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="1">
-        <f>IF(H10="One-Time", G10, G10*META!$B$1)</f>
+        <f>IF(H10="One-Time", G10,IF(H10="Weekly", G10*META!$B$2, G10*META!$B$1))</f>
         <v>1000</v>
       </c>
       <c r="J10">
@@ -1830,7 +1913,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I11" s="1">
-        <f>IF(H11="One-Time", G11, G11*META!$B$1)</f>
+        <f>IF(H11="One-Time", G11,IF(H11="Weekly", G11*META!$B$2, G11*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L11" s="1">
@@ -1844,7 +1927,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I12" s="1">
-        <f>IF(H12="One-Time", G12, G12*META!$B$1)</f>
+        <f>IF(H12="One-Time", G12,IF(H12="Weekly", G12*META!$B$2, G12*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L12" s="1">
@@ -1858,7 +1941,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I13" s="1">
-        <f>IF(H13="One-Time", G13, G13*META!$B$1)</f>
+        <f>IF(H13="One-Time", G13,IF(H13="Weekly", G13*META!$B$2, G13*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L13" s="1">
@@ -1872,7 +1955,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I14" s="1">
-        <f>IF(H14="One-Time", G14, G14*META!$B$1)</f>
+        <f>IF(H14="One-Time", G14,IF(H14="Weekly", G14*META!$B$2, G14*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L14" s="1">
@@ -1886,7 +1969,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I15" s="1">
-        <f>IF(H15="One-Time", G15, G15*META!$B$1)</f>
+        <f>IF(H15="One-Time", G15,IF(H15="Weekly", G15*META!$B$2, G15*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L15" s="1">
@@ -1900,7 +1983,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I16" s="1">
-        <f>IF(H16="One-Time", G16, G16*META!$B$1)</f>
+        <f>IF(H16="One-Time", G16,IF(H16="Weekly", G16*META!$B$2, G16*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L16" s="1">
@@ -1914,7 +1997,7 @@
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I17" s="1">
-        <f>IF(H17="One-Time", G17, G17*META!$B$1)</f>
+        <f>IF(H17="One-Time", G17,IF(H17="Weekly", G17*META!$B$2, G17*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L17" s="1">
@@ -1928,7 +2011,7 @@
     </row>
     <row r="18" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I18" s="1">
-        <f>IF(H18="One-Time", G18, G18*META!$B$1)</f>
+        <f>IF(H18="One-Time", G18,IF(H18="Weekly", G18*META!$B$2, G18*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L18" s="1">
@@ -1942,7 +2025,7 @@
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I19" s="1">
-        <f>IF(H19="One-Time", G19, G19*META!$B$1)</f>
+        <f>IF(H19="One-Time", G19,IF(H19="Weekly", G19*META!$B$2, G19*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L19" s="1">
@@ -1956,7 +2039,7 @@
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I20" s="1">
-        <f>IF(H20="One-Time", G20, G20*META!$B$1)</f>
+        <f>IF(H20="One-Time", G20,IF(H20="Weekly", G20*META!$B$2, G20*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L20" s="1">
@@ -1970,7 +2053,7 @@
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I21" s="1">
-        <f>IF(H21="One-Time", G21, G21*META!$B$1)</f>
+        <f>IF(H21="One-Time", G21,IF(H21="Weekly", G21*META!$B$2, G21*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L21" s="1">
@@ -1984,7 +2067,7 @@
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I22" s="1">
-        <f>IF(H22="One-Time", G22, G22*META!$B$1)</f>
+        <f>IF(H22="One-Time", G22,IF(H22="Weekly", G22*META!$B$2, G22*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L22" s="1">
@@ -1998,7 +2081,7 @@
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I23" s="1">
-        <f>IF(H23="One-Time", G23, G23*META!$B$1)</f>
+        <f>IF(H23="One-Time", G23,IF(H23="Weekly", G23*META!$B$2, G23*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L23" s="1">
@@ -2012,7 +2095,7 @@
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I24" s="1">
-        <f>IF(H24="One-Time", G24, G24*META!$B$1)</f>
+        <f>IF(H24="One-Time", G24,IF(H24="Weekly", G24*META!$B$2, G24*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L24" s="1">
@@ -2026,7 +2109,7 @@
     </row>
     <row r="25" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I25" s="1">
-        <f>IF(H25="One-Time", G25, G25*META!$B$1)</f>
+        <f>IF(H25="One-Time", G25,IF(H25="Weekly", G25*META!$B$2, G25*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L25" s="1">
@@ -2040,7 +2123,7 @@
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I26" s="1">
-        <f>IF(H26="One-Time", G26, G26*META!$B$1)</f>
+        <f>IF(H26="One-Time", G26,IF(H26="Weekly", G26*META!$B$2, G26*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L26" s="1">
@@ -2054,7 +2137,7 @@
     </row>
     <row r="27" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I27" s="1">
-        <f>IF(H27="One-Time", G27, G27*META!$B$1)</f>
+        <f>IF(H27="One-Time", G27,IF(H27="Weekly", G27*META!$B$2, G27*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L27" s="1">
@@ -2068,7 +2151,7 @@
     </row>
     <row r="28" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I28" s="1">
-        <f>IF(H28="One-Time", G28, G28*META!$B$1)</f>
+        <f>IF(H28="One-Time", G28,IF(H28="Weekly", G28*META!$B$2, G28*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L28" s="1">
@@ -2082,7 +2165,7 @@
     </row>
     <row r="29" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I29" s="1">
-        <f>IF(H29="One-Time", G29, G29*META!$B$1)</f>
+        <f>IF(H29="One-Time", G29,IF(H29="Weekly", G29*META!$B$2, G29*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L29" s="1">
@@ -2096,7 +2179,7 @@
     </row>
     <row r="30" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I30" s="1">
-        <f>IF(H30="One-Time", G30, G30*META!$B$1)</f>
+        <f>IF(H30="One-Time", G30,IF(H30="Weekly", G30*META!$B$2, G30*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L30" s="1">
@@ -2110,7 +2193,7 @@
     </row>
     <row r="31" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I31" s="1">
-        <f>IF(H31="One-Time", G31, G31*META!$B$1)</f>
+        <f>IF(H31="One-Time", G31,IF(H31="Weekly", G31*META!$B$2, G31*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L31" s="1">
@@ -2124,7 +2207,7 @@
     </row>
     <row r="32" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I32" s="1">
-        <f>IF(H32="One-Time", G32, G32*META!$B$1)</f>
+        <f>IF(H32="One-Time", G32,IF(H32="Weekly", G32*META!$B$2, G32*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L32" s="1">
@@ -2138,7 +2221,7 @@
     </row>
     <row r="33" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I33" s="1">
-        <f>IF(H33="One-Time", G33, G33*META!$B$1)</f>
+        <f>IF(H33="One-Time", G33,IF(H33="Weekly", G33*META!$B$2, G33*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L33" s="1">
@@ -2152,7 +2235,7 @@
     </row>
     <row r="34" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I34" s="1">
-        <f>IF(H34="One-Time", G34, G34*META!$B$1)</f>
+        <f>IF(H34="One-Time", G34,IF(H34="Weekly", G34*META!$B$2, G34*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L34" s="1">
@@ -2166,7 +2249,7 @@
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I35" s="1">
-        <f>IF(H35="One-Time", G35, G35*META!$B$1)</f>
+        <f>IF(H35="One-Time", G35,IF(H35="Weekly", G35*META!$B$2, G35*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L35" s="1">
@@ -2180,7 +2263,7 @@
     </row>
     <row r="36" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I36" s="1">
-        <f>IF(H36="One-Time", G36, G36*META!$B$1)</f>
+        <f>IF(H36="One-Time", G36,IF(H36="Weekly", G36*META!$B$2, G36*META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="L36" s="1">
@@ -2219,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CAFB97-75A0-9346-B6D1-9039BFF4C6BB}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2236,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -2257,21 +2340,21 @@
         <v>13</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="3">
         <v>43497</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4">
         <v>10000</v>
@@ -2280,22 +2363,22 @@
         <v>14</v>
       </c>
       <c r="I2" s="1">
-        <f>IF(H2="One-Time", G2, G2*META!$B$1)</f>
+        <f>IF(H2="One-Time", G2,IF(H2="Weekly", G2*META!$B$2, G2*META!$B$1))</f>
         <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="3">
         <v>43511</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="4">
         <v>10000</v>
@@ -2304,13 +2387,13 @@
         <v>14</v>
       </c>
       <c r="I3" s="1">
-        <f>IF(H3="One-Time", G3, G3*META!$B$1)</f>
+        <f>IF(H3="One-Time", G3,IF(H3="Weekly", G3*META!$B$2, G3*META!$B$1))</f>
         <v>10000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3">
         <v>43586</v>
@@ -2325,7 +2408,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="1">
-        <f>IF(H4="One-Time", G4, G4*META!$B$1)</f>
+        <f>IF(H4="One-Time", G4,IF(H4="Weekly", G4*META!$B$2, G4*META!$B$1))</f>
         <v>15000</v>
       </c>
     </row>
@@ -2334,7 +2417,7 @@
         <v>14</v>
       </c>
       <c r="I5" s="1">
-        <f>IF(H5="One-Time", G5, G5*META!$B$1)</f>
+        <f>IF(H5="One-Time", G5,IF(H5="Weekly", G5*META!$B$2, G5*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2343,7 +2426,7 @@
         <v>14</v>
       </c>
       <c r="I6" s="1">
-        <f>IF(H6="One-Time", G6, G6*META!$B$1)</f>
+        <f>IF(H6="One-Time", G6,IF(H6="Weekly", G6*META!$B$2, G6*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2352,7 +2435,7 @@
         <v>14</v>
       </c>
       <c r="I7" s="1">
-        <f>IF(H7="One-Time", G7, G7*META!$B$1)</f>
+        <f>IF(H7="One-Time", G7,IF(H7="Weekly", G7*META!$B$2, G7*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2361,7 +2444,7 @@
         <v>14</v>
       </c>
       <c r="I8" s="1">
-        <f>IF(H8="One-Time", G8, G8*META!$B$1)</f>
+        <f>IF(H8="One-Time", G8,IF(H8="Weekly", G8*META!$B$2, G8*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2370,7 +2453,7 @@
         <v>14</v>
       </c>
       <c r="I9" s="1">
-        <f>IF(H9="One-Time", G9, G9*META!$B$1)</f>
+        <f>IF(H9="One-Time", G9,IF(H9="Weekly", G9*META!$B$2, G9*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2379,7 +2462,7 @@
         <v>14</v>
       </c>
       <c r="I10" s="1">
-        <f>IF(H10="One-Time", G10, G10*META!$B$1)</f>
+        <f>IF(H10="One-Time", G10,IF(H10="Weekly", G10*META!$B$2, G10*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2388,7 +2471,7 @@
         <v>14</v>
       </c>
       <c r="I11" s="1">
-        <f>IF(H11="One-Time", G11, G11*META!$B$1)</f>
+        <f>IF(H11="One-Time", G11,IF(H11="Weekly", G11*META!$B$2, G11*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2397,7 +2480,7 @@
         <v>14</v>
       </c>
       <c r="I12" s="1">
-        <f>IF(H12="One-Time", G12, G12*META!$B$1)</f>
+        <f>IF(H12="One-Time", G12,IF(H12="Weekly", G12*META!$B$2, G12*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2406,7 +2489,7 @@
         <v>14</v>
       </c>
       <c r="I13" s="1">
-        <f>IF(H13="One-Time", G13, G13*META!$B$1)</f>
+        <f>IF(H13="One-Time", G13,IF(H13="Weekly", G13*META!$B$2, G13*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2415,7 +2498,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="1">
-        <f>IF(H14="One-Time", G14, G14*META!$B$1)</f>
+        <f>IF(H14="One-Time", G14,IF(H14="Weekly", G14*META!$B$2, G14*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2424,7 +2507,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="1">
-        <f>IF(H15="One-Time", G15, G15*META!$B$1)</f>
+        <f>IF(H15="One-Time", G15,IF(H15="Weekly", G15*META!$B$2, G15*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2433,7 +2516,7 @@
         <v>14</v>
       </c>
       <c r="I16" s="1">
-        <f>IF(H16="One-Time", G16, G16*META!$B$1)</f>
+        <f>IF(H16="One-Time", G16,IF(H16="Weekly", G16*META!$B$2, G16*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2442,7 +2525,7 @@
         <v>14</v>
       </c>
       <c r="I17" s="1">
-        <f>IF(H17="One-Time", G17, G17*META!$B$1)</f>
+        <f>IF(H17="One-Time", G17,IF(H17="Weekly", G17*META!$B$2, G17*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2451,7 +2534,7 @@
         <v>14</v>
       </c>
       <c r="I18" s="1">
-        <f>IF(H18="One-Time", G18, G18*META!$B$1)</f>
+        <f>IF(H18="One-Time", G18,IF(H18="Weekly", G18*META!$B$2, G18*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2460,7 +2543,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="1">
-        <f>IF(H19="One-Time", G19, G19*META!$B$1)</f>
+        <f>IF(H19="One-Time", G19,IF(H19="Weekly", G19*META!$B$2, G19*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2469,7 +2552,7 @@
         <v>14</v>
       </c>
       <c r="I20" s="1">
-        <f>IF(H20="One-Time", G20, G20*META!$B$1)</f>
+        <f>IF(H20="One-Time", G20,IF(H20="Weekly", G20*META!$B$2, G20*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2478,7 +2561,7 @@
         <v>14</v>
       </c>
       <c r="I21" s="1">
-        <f>IF(H21="One-Time", G21, G21*META!$B$1)</f>
+        <f>IF(H21="One-Time", G21,IF(H21="Weekly", G21*META!$B$2, G21*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2487,7 +2570,7 @@
         <v>14</v>
       </c>
       <c r="I22" s="1">
-        <f>IF(H22="One-Time", G22, G22*META!$B$1)</f>
+        <f>IF(H22="One-Time", G22,IF(H22="Weekly", G22*META!$B$2, G22*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2496,7 +2579,7 @@
         <v>14</v>
       </c>
       <c r="I23" s="1">
-        <f>IF(H23="One-Time", G23, G23*META!$B$1)</f>
+        <f>IF(H23="One-Time", G23,IF(H23="Weekly", G23*META!$B$2, G23*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2505,7 +2588,7 @@
         <v>14</v>
       </c>
       <c r="I24" s="1">
-        <f>IF(H24="One-Time", G24, G24*META!$B$1)</f>
+        <f>IF(H24="One-Time", G24,IF(H24="Weekly", G24*META!$B$2, G24*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2514,7 +2597,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="1">
-        <f>IF(H25="One-Time", G25, G25*META!$B$1)</f>
+        <f>IF(H25="One-Time", G25,IF(H25="Weekly", G25*META!$B$2, G25*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2523,7 +2606,7 @@
         <v>14</v>
       </c>
       <c r="I26" s="1">
-        <f>IF(H26="One-Time", G26, G26*META!$B$1)</f>
+        <f>IF(H26="One-Time", G26,IF(H26="Weekly", G26*META!$B$2, G26*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2532,7 +2615,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="1">
-        <f>IF(H27="One-Time", G27, G27*META!$B$1)</f>
+        <f>IF(H27="One-Time", G27,IF(H27="Weekly", G27*META!$B$2, G27*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2541,7 +2624,7 @@
         <v>14</v>
       </c>
       <c r="I28" s="1">
-        <f>IF(H28="One-Time", G28, G28*META!$B$1)</f>
+        <f>IF(H28="One-Time", G28,IF(H28="Weekly", G28*META!$B$2, G28*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2550,7 +2633,7 @@
         <v>14</v>
       </c>
       <c r="I29" s="1">
-        <f>IF(H29="One-Time", G29, G29*META!$B$1)</f>
+        <f>IF(H29="One-Time", G29,IF(H29="Weekly", G29*META!$B$2, G29*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2559,7 +2642,7 @@
         <v>14</v>
       </c>
       <c r="I30" s="1">
-        <f>IF(H30="One-Time", G30, G30*META!$B$1)</f>
+        <f>IF(H30="One-Time", G30,IF(H30="Weekly", G30*META!$B$2, G30*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2568,7 +2651,7 @@
         <v>14</v>
       </c>
       <c r="I31" s="1">
-        <f>IF(H31="One-Time", G31, G31*META!$B$1)</f>
+        <f>IF(H31="One-Time", G31,IF(H31="Weekly", G31*META!$B$2, G31*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2577,7 +2660,7 @@
         <v>14</v>
       </c>
       <c r="I32" s="1">
-        <f>IF(H32="One-Time", G32, G32*META!$B$1)</f>
+        <f>IF(H32="One-Time", G32,IF(H32="Weekly", G32*META!$B$2, G32*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2586,7 +2669,7 @@
         <v>14</v>
       </c>
       <c r="I33" s="1">
-        <f>IF(H33="One-Time", G33, G33*META!$B$1)</f>
+        <f>IF(H33="One-Time", G33,IF(H33="Weekly", G33*META!$B$2, G33*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2595,7 +2678,7 @@
         <v>14</v>
       </c>
       <c r="I34" s="1">
-        <f>IF(H34="One-Time", G34, G34*META!$B$1)</f>
+        <f>IF(H34="One-Time", G34,IF(H34="Weekly", G34*META!$B$2, G34*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2604,7 +2687,7 @@
         <v>14</v>
       </c>
       <c r="I35" s="1">
-        <f>IF(H35="One-Time", G35, G35*META!$B$1)</f>
+        <f>IF(H35="One-Time", G35,IF(H35="Weekly", G35*META!$B$2, G35*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2613,7 +2696,7 @@
         <v>14</v>
       </c>
       <c r="I36" s="1">
-        <f>IF(H36="One-Time", G36, G36*META!$B$1)</f>
+        <f>IF(H36="One-Time", G36,IF(H36="Weekly", G36*META!$B$2, G36*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2622,7 +2705,7 @@
         <v>14</v>
       </c>
       <c r="I37" s="1">
-        <f>IF(H37="One-Time", G37, G37*META!$B$1)</f>
+        <f>IF(H37="One-Time", G37,IF(H37="Weekly", G37*META!$B$2, G37*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2631,7 +2714,7 @@
         <v>14</v>
       </c>
       <c r="I38" s="1">
-        <f>IF(H38="One-Time", G38, G38*META!$B$1)</f>
+        <f>IF(H38="One-Time", G38,IF(H38="Weekly", G38*META!$B$2, G38*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2640,7 +2723,7 @@
         <v>14</v>
       </c>
       <c r="I39" s="1">
-        <f>IF(H39="One-Time", G39, G39*META!$B$1)</f>
+        <f>IF(H39="One-Time", G39,IF(H39="Weekly", G39*META!$B$2, G39*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2649,7 +2732,7 @@
         <v>14</v>
       </c>
       <c r="I40" s="1">
-        <f>IF(H40="One-Time", G40, G40*META!$B$1)</f>
+        <f>IF(H40="One-Time", G40,IF(H40="Weekly", G40*META!$B$2, G40*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2686,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78948E2-0627-B441-AE13-F68FE46A5720}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="C1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2707,7 +2790,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -2728,7 +2811,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -2736,7 +2819,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2745,7 +2828,7 @@
         <v>43466</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2754,10 +2837,10 @@
         <v>4000</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1">
-        <f>IF(H2="One-Time", G2,G2*META!$B$1)</f>
+        <f>IF(H2="One-Time", G2,IF(H2="Weekly", G2*META!$B$2, G2*META!$B$1))</f>
         <v>20000</v>
       </c>
     </row>
@@ -2766,7 +2849,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -2784,118 +2867,118 @@
         <v>500</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1">
-        <f>IF(H3="One-Time", G3,G3*META!$B$1)</f>
-        <v>2500</v>
+        <f>IF(H3="One-Time", G3,IF(H3="Weekly", G3*META!$B$2, G3*META!$B$1))</f>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I4" s="1">
-        <f>IF(H4="One-Time", G4,G4*META!$B$1)</f>
+        <f>IF(H4="One-Time", G4,IF(H4="Weekly", G4*META!$B$2, G4*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I5" s="1">
-        <f>IF(H5="One-Time", G5,G5*META!$B$1)</f>
+        <f>IF(H5="One-Time", G5,IF(H5="Weekly", G5*META!$B$2, G5*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I6" s="1">
-        <f>IF(H6="One-Time", G6,G6*META!$B$1)</f>
+        <f>IF(H6="One-Time", G6,IF(H6="Weekly", G6*META!$B$2, G6*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I7" s="1">
-        <f>IF(H7="One-Time", G7,G7*META!$B$1)</f>
+        <f>IF(H7="One-Time", G7,IF(H7="Weekly", G7*META!$B$2, G7*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I8" s="1">
-        <f>IF(H8="One-Time", G8,G8*META!$B$1)</f>
+        <f>IF(H8="One-Time", G8,IF(H8="Weekly", G8*META!$B$2, G8*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I9" s="1">
-        <f>IF(H9="One-Time", G9,G9*META!$B$1)</f>
+        <f>IF(H9="One-Time", G9,IF(H9="Weekly", G9*META!$B$2, G9*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I10" s="1">
-        <f>IF(H10="One-Time", G10,G10*META!$B$1)</f>
+        <f>IF(H10="One-Time", G10,IF(H10="Weekly", G10*META!$B$2, G10*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I11" s="1">
-        <f>IF(H11="One-Time", G11,G11*META!$B$1)</f>
+        <f>IF(H11="One-Time", G11,IF(H11="Weekly", G11*META!$B$2, G11*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I12" s="1">
-        <f>IF(H12="One-Time", G12,G12*META!$B$1)</f>
+        <f>IF(H12="One-Time", G12,IF(H12="Weekly", G12*META!$B$2, G12*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I13" s="1">
-        <f>IF(H13="One-Time", G13,G13*META!$B$1)</f>
+        <f>IF(H13="One-Time", G13,IF(H13="Weekly", G13*META!$B$2, G13*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I14" s="1">
-        <f>IF(H14="One-Time", G14,G14*META!$B$1)</f>
+        <f>IF(H14="One-Time", G14,IF(H14="Weekly", G14*META!$B$2, G14*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I15" s="1">
-        <f>IF(H15="One-Time", G15,G15*META!$B$1)</f>
+        <f>IF(H15="One-Time", G15,IF(H15="Weekly", G15*META!$B$2, G15*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I16" s="1">
-        <f>IF(H16="One-Time", G16,G16*META!$B$1)</f>
+        <f>IF(H16="One-Time", G16,IF(H16="Weekly", G16*META!$B$2, G16*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I17" s="1">
-        <f>IF(H17="One-Time", G17,G17*META!$B$1)</f>
+        <f>IF(H17="One-Time", G17,IF(H17="Weekly", G17*META!$B$2, G17*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I18" s="1">
-        <f>IF(H18="One-Time", G18,G18*META!$B$1)</f>
+        <f>IF(H18="One-Time", G18,IF(H18="Weekly", G18*META!$B$2, G18*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I19" s="1">
-        <f>IF(H19="One-Time", G19,G19*META!$B$1)</f>
+        <f>IF(H19="One-Time", G19,IF(H19="Weekly", G19*META!$B$2, G19*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I20" s="1">
-        <f>IF(H20="One-Time", G20,G20*META!$B$1)</f>
+        <f>IF(H20="One-Time", G20,IF(H20="Weekly", G20*META!$B$2, G20*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I21" s="1">
-        <f>IF(H21="One-Time", G21,G21*META!$B$1)</f>
+        <f>IF(H21="One-Time", G21,IF(H21="Weekly", G21*META!$B$2, G21*META!$B$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -2930,10 +3013,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF870036-DF5B-FD43-96B7-9E1C1C631AB4}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2942,14 +3025,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>27</v>
+      <c r="A1" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B1">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2957,6 +3040,24 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <f>B1*4</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3">
+        <f>B2*7</f>
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2965,10 +3066,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED54123-DF30-A242-B592-72A99EBCF2D6}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2981,7 +3082,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -2992,18 +3093,18 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3011,12 +3112,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3028,8 +3124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D7D8B-99CC-1E4C-A66C-7B87E4EAC53A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3039,15 +3135,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
-      </c>
-      <c r="B1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>1</v>

</xml_diff>